<commit_message>
Follow channel testcases added
</commit_message>
<xml_diff>
--- a/src/main/resources/configfile/Kisan.NetTestData.xlsx
+++ b/src/main/resources/configfile/Kisan.NetTestData.xlsx
@@ -7,6 +7,7 @@
     <sheet state="visible" name="Invite To Download App" sheetId="2" r:id="rId4"/>
     <sheet state="visible" name="Invite To Follow Channel" sheetId="3" r:id="rId5"/>
     <sheet state="visible" name="Search Channels" sheetId="4" r:id="rId6"/>
+    <sheet state="visible" name="Follow Channels" sheetId="5" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="16">
   <si>
     <t>UserName</t>
   </si>
@@ -37,28 +38,31 @@
     <t>Y</t>
   </si>
   <si>
+    <t>UserNameStart</t>
+  </si>
+  <si>
     <t>ChannelName</t>
   </si>
   <si>
+    <t>exhibit_94@mailinator.com</t>
+  </si>
+  <si>
+    <t>chan@kisan18</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>KISAN</t>
+  </si>
+  <si>
     <t>Existing</t>
   </si>
   <si>
-    <t>KISAN</t>
-  </si>
-  <si>
     <t>abcdefghijklm</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>UserNameStart</t>
-  </si>
-  <si>
-    <t>exhibit_94@mailinator.com</t>
-  </si>
-  <si>
-    <t>chan@kisan18</t>
+    <t>FCI Magazine</t>
   </si>
 </sst>
 </file>
@@ -147,6 +151,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
@@ -159,7 +167,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -170,10 +178,10 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -256,7 +264,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -273,7 +281,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>9.021633629E9</v>
@@ -305,10 +313,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -322,7 +330,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
@@ -339,12 +347,55 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>